<commit_message>
UPDATE TDS + NEW DOC USER
</commit_message>
<xml_diff>
--- a/assets/Documents/Stage/Tableau de synthèse - Epreuve E4 - BTS SIO 2023.xlsx
+++ b/assets/Documents/Stage/Tableau de synthèse - Epreuve E4 - BTS SIO 2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flore\Desktop\Cours\Portfolio\portfolio-bernier-florent\assets\Documents\Stage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84F90777-1D95-484E-9890-49CB044159D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B571AED-BFBF-46BE-8013-B8CCC46639BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9360" yWindow="1905" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tableau de synthèse des réalisations professionnelles </t>
-  </si>
-  <si>
-    <t xml:space="preserve">N° candidat : </t>
   </si>
   <si>
     <t>Option :</t>
@@ -192,19 +189,37 @@
     <t>Mise en place d'un flux RSS (Google Alert/ Feedly)</t>
   </si>
   <si>
-    <t>AP3 - Mise en place d'une infrastructure mobile (Flutter)</t>
-  </si>
-  <si>
     <t>AP3 - Mise en place de l'infrastructure web (ReactJS)</t>
   </si>
   <si>
-    <t>Du XX/01/24 au XX/XX/24</t>
+    <t>AP3 - Mise en place d'une API (Javascript)</t>
   </si>
   <si>
-    <t>Du XX/10/23 au XX/01/24</t>
+    <t>AP4 - Mise en place d'une infrastructure mobile (Flutter)</t>
   </si>
   <si>
-    <t>AP3 - Mise en place d'une API (Javascript)</t>
+    <t>Du 18/01/24 au XX/XX/24</t>
+  </si>
+  <si>
+    <t>N° candidat : 02341334732</t>
+  </si>
+  <si>
+    <t>Du 09/10/23 au 15/01/24</t>
+  </si>
+  <si>
+    <t>Du 09/10/24 au 15/01/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pabete - Amélioration de la page inscription </t>
+  </si>
+  <si>
+    <t>Du 05/02/24 au 23/02/24</t>
+  </si>
+  <si>
+    <t>Pabete - Amélioration de la recherche de professionnel</t>
+  </si>
+  <si>
+    <t>Du 23/02/24 au xx/xx/24</t>
   </si>
 </sst>
 </file>
@@ -741,14 +756,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -781,30 +820,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2129,16 +2144,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>4421</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>17293</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>25743</xdr:rowOff>
+      <xdr:rowOff>12872</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>324</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>2300</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>13195</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>491422</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2153,7 +2168,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7946212" y="11121081"/>
+          <a:off x="6723408" y="11108210"/>
           <a:ext cx="1231578" cy="478550"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2179,16 +2194,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>12872</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>25743</xdr:rowOff>
+      <xdr:rowOff>12872</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>2</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>12873</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>492513</xdr:rowOff>
+      <xdr:rowOff>479642</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2203,7 +2218,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="7941791" y="11121081"/>
+          <a:off x="6718987" y="11108210"/>
           <a:ext cx="1235677" cy="466770"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2905,6 +2920,406 @@
         <a:xfrm flipV="1">
           <a:off x="11648818" y="12601318"/>
           <a:ext cx="1235677" cy="466770"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>15918</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2296</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>478550</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Connecteur droit 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FB0BB7F-07E5-4691-987B-D3A2A23EEE65}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11664736" y="14338986"/>
+          <a:ext cx="1222053" cy="478550"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>466770</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5B79671-9E6F-4324-BDF2-63E9F9B4A73D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11648818" y="14338986"/>
+          <a:ext cx="1235676" cy="466770"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>15918</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2296</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>478550</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Connecteur droit 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{932383F7-89FD-49E8-B9EB-EC03F2857D12}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11664736" y="14840980"/>
+          <a:ext cx="1222053" cy="478550"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>466770</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE8A2BEE-E481-4543-999F-3924505517CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11648818" y="14840980"/>
+          <a:ext cx="1235676" cy="466770"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>15918</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2295</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>478550</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Connecteur droit 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F73A04D-45E2-4BFE-B3D7-F5402CEEEF94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10429060" y="14338986"/>
+          <a:ext cx="1222053" cy="478550"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>466770</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76CACB02-C059-4EBB-92CB-F7D8BF671B5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10413142" y="14338986"/>
+          <a:ext cx="1235676" cy="466770"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>15918</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2295</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>478550</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="50" name="Connecteur droit 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D813D7D1-0A4E-4CD4-BCC0-F994A779928B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10429060" y="14840980"/>
+          <a:ext cx="1222053" cy="478550"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>466770</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{127EAE31-F3A9-4008-8DC2-49A87ED93133}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10413142" y="14840980"/>
+          <a:ext cx="1235676" cy="466770"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3222,8 +3637,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="74" zoomScaleNormal="294" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="74" zoomScaleNormal="294" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3236,124 +3651,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="24"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
-        <v>26</v>
+      <c r="A3" s="23" t="s">
+        <v>25</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="42" t="s">
-        <v>3</v>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="29" t="s">
+        <v>48</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="43"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="30"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="39" t="s">
-        <v>27</v>
+      <c r="A4" s="26" t="s">
+        <v>26</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="41"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="28"/>
       <c r="F4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="H4" s="19" t="s">
         <v>5</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
-        <v>28</v>
+      <c r="A5" s="41" t="s">
+        <v>27</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="35"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="43"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="C6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="32"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="40"/>
       <c r="C7" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="E7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="F7" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="G7" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="H7" s="21" t="s">
         <v>19</v>
-      </c>
-      <c r="H7" s="21" t="s">
-        <v>20</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -3392,16 +3807,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="25" t="s">
-        <v>21</v>
+      <c r="A8" s="33" t="s">
+        <v>20</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="27"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="35"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -3440,10 +3855,10 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="15"/>
@@ -3489,10 +3904,10 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
@@ -3538,10 +3953,10 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -3587,10 +4002,10 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -3636,10 +4051,10 @@
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -3685,10 +4100,10 @@
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
@@ -3734,10 +4149,10 @@
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -3783,10 +4198,10 @@
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -3832,9 +4247,11 @@
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
-      <c r="B17" s="8"/>
+      <c r="B17" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
@@ -3879,10 +4296,10 @@
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -3927,16 +4344,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="28" t="s">
-        <v>22</v>
+      <c r="A19" s="36" t="s">
+        <v>21</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="30"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="38"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -3975,10 +4392,10 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
@@ -4024,10 +4441,10 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
@@ -4072,8 +4489,12 @@
       <c r="AQ21"/>
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
-      <c r="B22" s="8"/>
+      <c r="A22" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
@@ -4117,8 +4538,12 @@
       <c r="AQ22"/>
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
-      <c r="B23" s="8"/>
+      <c r="A23" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
@@ -4297,16 +4722,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="28" t="s">
-        <v>23</v>
+      <c r="A27" s="36" t="s">
+        <v>22</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="30"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="38"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -4751,11 +5176,6 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -4763,73 +5183,22 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="48" orientation="portrait"/>
+  <pageSetup paperSize="9" scale="48" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <CultureName xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <LMS_Mappings xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <Owner xmlns="a54630e7-b857-4bdf-808b-f1da7c130004">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Has_Teacher_Only_SectionGroup xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <TeamsChannelId xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <Invited_Teachers xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <NotebookType xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <Distribution_Groups xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a54630e7-b857-4bdf-808b-f1da7c130004">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Templates xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <TaxCatchAll xmlns="57e91659-be1d-4d29-8a34-37188ca8e23d" xsi:nil="true"/>
-    <AppVersion xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <Math_Settings xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <Teams_Channel_Section_Location xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <Invited_Students xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <FolderType xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <Teachers xmlns="a54630e7-b857-4bdf-808b-f1da7c130004">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <Students xmlns="a54630e7-b857-4bdf-808b-f1da7c130004">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <Student_Groups xmlns="a54630e7-b857-4bdf-808b-f1da7c130004">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002338DD58AC86894E92A5BEFCB2D30A8D" ma:contentTypeVersion="34" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6b073224b491898f5bb610979279e59c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a54630e7-b857-4bdf-808b-f1da7c130004" xmlns:ns3="57e91659-be1d-4d29-8a34-37188ca8e23d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f2c6147616482782723debbc5b2f32a" ns2:_="" ns3:_="">
     <xsd:import namespace="a54630e7-b857-4bdf-808b-f1da7c130004"/>
@@ -5246,6 +5615,62 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <CultureName xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <LMS_Mappings xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <Owner xmlns="a54630e7-b857-4bdf-808b-f1da7c130004">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Has_Teacher_Only_SectionGroup xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <TeamsChannelId xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <Invited_Teachers xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <NotebookType xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <Distribution_Groups xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a54630e7-b857-4bdf-808b-f1da7c130004">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Templates xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <TaxCatchAll xmlns="57e91659-be1d-4d29-8a34-37188ca8e23d" xsi:nil="true"/>
+    <AppVersion xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <Math_Settings xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <Teams_Channel_Section_Location xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <Invited_Students xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <FolderType xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <Teachers xmlns="a54630e7-b857-4bdf-808b-f1da7c130004">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <Students xmlns="a54630e7-b857-4bdf-808b-f1da7c130004">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <Student_Groups xmlns="a54630e7-b857-4bdf-808b-f1da7c130004">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5256,23 +5681,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14A1D336-8C6A-4F82-BD4C-ECADBE989409}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="57e91659-be1d-4d29-8a34-37188ca8e23d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="a54630e7-b857-4bdf-808b-f1da7c130004"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B284ED27-3496-42FE-8F98-11549EA57EF1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5291,6 +5699,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14A1D336-8C6A-4F82-BD4C-ECADBE989409}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="57e91659-be1d-4d29-8a34-37188ca8e23d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="a54630e7-b857-4bdf-808b-f1da7c130004"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BF4CA8B-910A-4F71-9526-D749B61C44AF}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
UPDATE AP4 DOCUMENTS + TABLEAU DE SYNTHESE
</commit_message>
<xml_diff>
--- a/assets/Documents/Stage/Tableau de synthèse - Epreuve E4 - BTS SIO 2023.xlsx
+++ b/assets/Documents/Stage/Tableau de synthèse - Epreuve E4 - BTS SIO 2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flore\Desktop\Cours\Portfolio\portfolio-bernier-florent\assets\Documents\Stage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B571AED-BFBF-46BE-8013-B8CCC46639BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE098D1-2642-49FB-9C05-1E195991D2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9360" yWindow="1905" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
-  </si>
-  <si>
-    <t>SESSION 2023</t>
   </si>
   <si>
     <t xml:space="preserve">Tableau de synthèse des réalisations professionnelles </t>
@@ -192,13 +189,7 @@
     <t>AP3 - Mise en place de l'infrastructure web (ReactJS)</t>
   </si>
   <si>
-    <t>AP3 - Mise en place d'une API (Javascript)</t>
-  </si>
-  <si>
     <t>AP4 - Mise en place d'une infrastructure mobile (Flutter)</t>
-  </si>
-  <si>
-    <t>Du 18/01/24 au XX/XX/24</t>
   </si>
   <si>
     <t>N° candidat : 02341334732</t>
@@ -219,7 +210,16 @@
     <t>Pabete - Amélioration de la recherche de professionnel</t>
   </si>
   <si>
-    <t>Du 23/02/24 au xx/xx/24</t>
+    <t>AP3 et AP4 - Mise en place d'une API (Javascript)</t>
+  </si>
+  <si>
+    <t>Du 18/01/24 au 25/04/24</t>
+  </si>
+  <si>
+    <t>Du 23/02/24 au 08/03/24</t>
+  </si>
+  <si>
+    <t>SESSION 2024</t>
   </si>
 </sst>
 </file>
@@ -756,38 +756,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -820,6 +796,30 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2946,21 +2946,21 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>15918</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2296</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>478550</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="2" name="Connecteur droit 5">
+        <xdr:cNvPr id="52" name="Connecteur droit 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FB0BB7F-07E5-4691-987B-D3A2A23EEE65}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{577F0423-7D9A-47D8-B90C-CB97EFEA54A4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2996,21 +2996,21 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>466770</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Connecteur droit 6">
+        <xdr:cNvPr id="53" name="Connecteur droit 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5B79671-9E6F-4324-BDF2-63E9F9B4A73D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B0E383B-6E03-417C-BA5D-71101BB10C32}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3046,21 +3046,21 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>15918</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2296</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>478550</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="10" name="Connecteur droit 5">
+        <xdr:cNvPr id="54" name="Connecteur droit 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{932383F7-89FD-49E8-B9EB-EC03F2857D12}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0008C22-E9DD-47B2-BAD3-8A3B30678C05}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3096,21 +3096,21 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>466770</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="11" name="Connecteur droit 6">
+        <xdr:cNvPr id="55" name="Connecteur droit 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE8A2BEE-E481-4543-999F-3924505517CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7543F15F-B07D-48DC-BB4C-407299506BE3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3146,21 +3146,21 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>15918</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>2295</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>478550</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="32" name="Connecteur droit 5">
+        <xdr:cNvPr id="56" name="Connecteur droit 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F73A04D-45E2-4BFE-B3D7-F5402CEEEF94}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99DCBC50-FD56-4120-8F4A-3CA20806B852}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3196,21 +3196,21 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>466770</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="33" name="Connecteur droit 6">
+        <xdr:cNvPr id="57" name="Connecteur droit 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76CACB02-C059-4EBB-92CB-F7D8BF671B5C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EF7AC79-4081-452C-9525-F9B53CDB78A5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3246,21 +3246,21 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>15918</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>2295</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>478550</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="50" name="Connecteur droit 5">
+        <xdr:cNvPr id="58" name="Connecteur droit 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D813D7D1-0A4E-4CD4-BCC0-F994A779928B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4308D55E-57FE-402B-AE56-C1AA01A9E273}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3296,21 +3296,21 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>466770</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="51" name="Connecteur droit 6">
+        <xdr:cNvPr id="59" name="Connecteur droit 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{127EAE31-F3A9-4008-8DC2-49A87ED93133}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A621F0D-AFDA-451B-90E3-6756D6460963}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3637,8 +3637,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="74" zoomScaleNormal="294" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="74" zoomScaleNormal="294" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3651,124 +3651,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="24"/>
+    </row>
+    <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="22"/>
-    </row>
-    <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
-        <v>25</v>
+      <c r="A3" s="36" t="s">
+        <v>24</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="29" t="s">
-        <v>48</v>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="42" t="s">
+        <v>45</v>
       </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="30"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="43"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
-        <v>26</v>
+      <c r="A4" s="39" t="s">
+        <v>25</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="41"/>
       <c r="F4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="H4" s="19" t="s">
         <v>4</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
-        <v>27</v>
+      <c r="A5" s="33" t="s">
+        <v>26</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="43"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="40"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="E7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="F7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="G7" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="H7" s="21" t="s">
         <v>18</v>
-      </c>
-      <c r="H7" s="21" t="s">
-        <v>19</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -3807,16 +3807,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="33" t="s">
-        <v>20</v>
+      <c r="A8" s="25" t="s">
+        <v>19</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="35"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="27"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -3855,10 +3855,10 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="15"/>
@@ -3904,10 +3904,10 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
@@ -3953,10 +3953,10 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -4002,10 +4002,10 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -4051,10 +4051,10 @@
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -4100,10 +4100,10 @@
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
@@ -4149,10 +4149,10 @@
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -4198,10 +4198,10 @@
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -4247,10 +4247,10 @@
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -4296,10 +4296,10 @@
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -4344,16 +4344,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="36" t="s">
-        <v>21</v>
+      <c r="A19" s="28" t="s">
+        <v>20</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="38"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="30"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -4392,10 +4392,10 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
@@ -4441,10 +4441,10 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
@@ -4489,12 +4489,8 @@
       <c r="AQ21"/>
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>52</v>
-      </c>
+      <c r="A22" s="9"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
@@ -4538,12 +4534,8 @@
       <c r="AQ22"/>
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>54</v>
-      </c>
+      <c r="A23" s="9"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
@@ -4722,16 +4714,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="36" t="s">
-        <v>22</v>
+      <c r="A27" s="28" t="s">
+        <v>21</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="38"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="30"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -4769,8 +4761,12 @@
       <c r="AQ27"/>
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="9"/>
-      <c r="B28" s="8"/>
+      <c r="A28" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
       <c r="E28" s="15"/>
@@ -4814,8 +4810,12 @@
       <c r="AQ28"/>
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9"/>
-      <c r="B29" s="8"/>
+      <c r="A29" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
@@ -5176,6 +5176,11 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -5183,11 +5188,6 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -5199,6 +5199,62 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <CultureName xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <LMS_Mappings xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <Owner xmlns="a54630e7-b857-4bdf-808b-f1da7c130004">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Has_Teacher_Only_SectionGroup xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <TeamsChannelId xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <Invited_Teachers xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <NotebookType xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <Distribution_Groups xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a54630e7-b857-4bdf-808b-f1da7c130004">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Templates xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <TaxCatchAll xmlns="57e91659-be1d-4d29-8a34-37188ca8e23d" xsi:nil="true"/>
+    <AppVersion xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <Math_Settings xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <Teams_Channel_Section_Location xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <Invited_Students xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <FolderType xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
+    <Teachers xmlns="a54630e7-b857-4bdf-808b-f1da7c130004">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <Students xmlns="a54630e7-b857-4bdf-808b-f1da7c130004">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <Student_Groups xmlns="a54630e7-b857-4bdf-808b-f1da7c130004">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002338DD58AC86894E92A5BEFCB2D30A8D" ma:contentTypeVersion="34" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6b073224b491898f5bb610979279e59c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a54630e7-b857-4bdf-808b-f1da7c130004" xmlns:ns3="57e91659-be1d-4d29-8a34-37188ca8e23d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f2c6147616482782723debbc5b2f32a" ns2:_="" ns3:_="">
     <xsd:import namespace="a54630e7-b857-4bdf-808b-f1da7c130004"/>
@@ -5615,62 +5671,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <CultureName xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <LMS_Mappings xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <Owner xmlns="a54630e7-b857-4bdf-808b-f1da7c130004">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Has_Teacher_Only_SectionGroup xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <TeamsChannelId xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <Invited_Teachers xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <NotebookType xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <Distribution_Groups xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a54630e7-b857-4bdf-808b-f1da7c130004">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Templates xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <TaxCatchAll xmlns="57e91659-be1d-4d29-8a34-37188ca8e23d" xsi:nil="true"/>
-    <AppVersion xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <Math_Settings xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <Teams_Channel_Section_Location xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <Invited_Students xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <FolderType xmlns="a54630e7-b857-4bdf-808b-f1da7c130004" xsi:nil="true"/>
-    <Teachers xmlns="a54630e7-b857-4bdf-808b-f1da7c130004">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <Students xmlns="a54630e7-b857-4bdf-808b-f1da7c130004">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <Student_Groups xmlns="a54630e7-b857-4bdf-808b-f1da7c130004">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5681,6 +5681,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14A1D336-8C6A-4F82-BD4C-ECADBE989409}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="57e91659-be1d-4d29-8a34-37188ca8e23d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="a54630e7-b857-4bdf-808b-f1da7c130004"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B284ED27-3496-42FE-8F98-11549EA57EF1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5699,23 +5716,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14A1D336-8C6A-4F82-BD4C-ECADBE989409}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="57e91659-be1d-4d29-8a34-37188ca8e23d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="a54630e7-b857-4bdf-808b-f1da7c130004"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BF4CA8B-910A-4F71-9526-D749B61C44AF}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
UPDATE AP4 + STAGE
</commit_message>
<xml_diff>
--- a/assets/Documents/Stage/Tableau de synthèse - Epreuve E4 - BTS SIO 2023.xlsx
+++ b/assets/Documents/Stage/Tableau de synthèse - Epreuve E4 - BTS SIO 2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flore\Desktop\Cours\Portfolio\portfolio-bernier-florent\assets\Documents\Stage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE098D1-2642-49FB-9C05-1E195991D2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC6FA46-5724-47BF-AB51-817CF274AFAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -141,9 +141,6 @@
     <t>Du 26/10/2022 au 13/01/2023</t>
   </si>
   <si>
-    <t>Du 10/2022 à maintenant</t>
-  </si>
-  <si>
     <t>Gestion de son réseau professionnel LinkedIn</t>
   </si>
   <si>
@@ -154,9 +151,6 @@
   </si>
   <si>
     <t>Du 03/2023 au 05/2023</t>
-  </si>
-  <si>
-    <t>Du 04/2023 à maintenant</t>
   </si>
   <si>
     <t>Team Vitality - Réalisation d'un projet de cybersécurité (phishing)</t>
@@ -195,16 +189,7 @@
     <t>N° candidat : 02341334732</t>
   </si>
   <si>
-    <t>Du 09/10/23 au 15/01/24</t>
-  </si>
-  <si>
-    <t>Du 09/10/24 au 15/01/24</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pabete - Amélioration de la page inscription </t>
-  </si>
-  <si>
-    <t>Du 05/02/24 au 23/02/24</t>
   </si>
   <si>
     <t>Pabete - Amélioration de la recherche de professionnel</t>
@@ -213,13 +198,28 @@
     <t>AP3 et AP4 - Mise en place d'une API (Javascript)</t>
   </si>
   <si>
-    <t>Du 18/01/24 au 25/04/24</t>
+    <t>SESSION 2024</t>
   </si>
   <si>
-    <t>Du 23/02/24 au 08/03/24</t>
+    <t>Du 18/01/2024 au 25/04/2024</t>
   </si>
   <si>
-    <t>SESSION 2024</t>
+    <t>Du 09/10/2024 au 15/01/2024</t>
+  </si>
+  <si>
+    <t>Du 09/10/2023 au 15/01/2024</t>
+  </si>
+  <si>
+    <t>Du 05/02/2024 au 23/02/2024</t>
+  </si>
+  <si>
+    <t>Du 23/02/2024 au 08/03/2024</t>
+  </si>
+  <si>
+    <t>Du 10/2022 au 31/05/2024</t>
+  </si>
+  <si>
+    <t>Du 04/2023 au 31/05/2024</t>
   </si>
 </sst>
 </file>
@@ -3637,8 +3637,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="74" zoomScaleNormal="294" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="74" zoomScaleNormal="294" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3660,7 +3660,7 @@
       <c r="E1" s="24"/>
       <c r="F1" s="24"/>
       <c r="G1" s="24" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H1" s="24"/>
     </row>
@@ -3685,7 +3685,7 @@
       <c r="D3" s="37"/>
       <c r="E3" s="38"/>
       <c r="F3" s="42" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G3" s="37"/>
       <c r="H3" s="43"/>
@@ -3855,7 +3855,7 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>27</v>
@@ -3953,10 +3953,10 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -4002,10 +4002,10 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -4051,10 +4051,10 @@
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -4100,10 +4100,10 @@
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
@@ -4149,10 +4149,10 @@
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -4198,10 +4198,10 @@
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -4247,10 +4247,10 @@
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -4296,10 +4296,10 @@
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -4392,10 +4392,10 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
@@ -4441,10 +4441,10 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
@@ -4762,10 +4762,10 @@
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
@@ -4811,10 +4811,10 @@
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>

</xml_diff>